<commit_message>
reset procfile to app from app2a
</commit_message>
<xml_diff>
--- a/todo_postgres_setup.xlsx
+++ b/todo_postgres_setup.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>conda create -n todo python=3.6</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>heroku config --app bhver2</t>
+  </si>
+  <si>
+    <t>heroku git:remote -a bhver2</t>
+  </si>
+  <si>
+    <t>use app2.py to run locally , app.py runs on heroku</t>
   </si>
 </sst>
 </file>
@@ -250,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -265,6 +271,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72:B79"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -778,68 +785,78 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B63" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B62" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B64" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" t="s">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="5" t="s">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="5" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B74" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>